<commit_message>
add interface for filter module
</commit_message>
<xml_diff>
--- a/Publishers.xlsx
+++ b/Publishers.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dongchen/git/Vianden/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="23560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="28">
   <si>
     <t>Title</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -46,10 +41,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DatabaseType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Abstract</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -110,10 +101,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Ieee</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Springer</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -132,6 +119,15 @@
   <si>
     <t>IET</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>PublisherType</t>
+  </si>
+  <si>
+    <t>Author Affiliations</t>
+  </si>
+  <si>
+    <t>IEEE</t>
   </si>
 </sst>
 </file>
@@ -144,7 +140,6 @@
       <color theme="1"/>
       <name val="DengXian"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -253,7 +248,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -308,7 +303,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="DengXian Light" panose="020F0302020204030204"/>
+        <a:latin typeface="DengXian Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -343,7 +338,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="DengXian" panose="020F0502020204030204"/>
+        <a:latin typeface="DengXian"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -520,7 +515,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -528,346 +523,362 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="7" max="7" width="14.5" customWidth="1"/>
+    <col min="4" max="4" width="17.375" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>12</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4" t="s">
+      <c r="J2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="4" t="s">
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="L10" s="5"/>
+      <c r="M10" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K10" s="5"/>
-      <c r="L10" s="6" t="s">
+    <row r="11" spans="1:14">
+      <c r="L11" s="7"/>
+      <c r="M11" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K11" s="7"/>
-      <c r="L11" s="6" t="s">
+    <row r="12" spans="1:14">
+      <c r="L12" s="8"/>
+      <c r="M12" s="6" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K12" s="8"/>
-      <c r="L12" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>